<commit_message>
Update RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES-MEUS.xlsx
</commit_message>
<xml_diff>
--- a/RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES-MEUS.xlsx
+++ b/RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES-MEUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos.brumatti\Documents\GitHub\patrimonio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C97E4-0F83-4274-96ED-8A382D39480C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41A69DD-A113-4FCA-9BBA-002DFDAC2889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="159">
   <si>
     <t>RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES</t>
   </si>
@@ -928,9 +928,9 @@
   </sheetPr>
   <dimension ref="A1:O214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,7 +2225,9 @@
       <c r="N42" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O42" s="2"/>
+      <c r="O42" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -2381,7 +2383,9 @@
       <c r="N46" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O46" s="2"/>
+      <c r="O46" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="47" spans="1:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -2713,7 +2717,9 @@
       <c r="N57" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O57" s="2"/>
+      <c r="O57" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="58" spans="1:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -2808,7 +2814,9 @@
       <c r="N60" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O60" s="2"/>
+      <c r="O60" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="61" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
@@ -2847,7 +2855,9 @@
       <c r="N61" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O61" s="2"/>
+      <c r="O61" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="62" spans="1:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">

</xml_diff>